<commit_message>
Modified Signin Test data
</commit_message>
<xml_diff>
--- a/Resources/TestData/qat03.xlsx
+++ b/Resources/TestData/qat03.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="REG" sheetId="4" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="509" uniqueCount="242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="509" uniqueCount="243">
   <si>
     <t>TC_NO</t>
   </si>
@@ -566,9 +566,6 @@
     <t>9191</t>
   </si>
   <si>
-    <t>ftrfrank1+automation2@gmail.com</t>
-  </si>
-  <si>
     <t>219-324-3764-102891-5</t>
   </si>
   <si>
@@ -753,6 +750,12 @@
   </si>
   <si>
     <t>https://frontier.com/corporate/news/home</t>
+  </si>
+  <si>
+    <t>ftrqat03+3@gmail.com</t>
+  </si>
+  <si>
+    <t>Password123</t>
   </si>
 </sst>
 </file>
@@ -926,7 +929,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -978,6 +981,7 @@
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1346,13 +1350,13 @@
         <v>159</v>
       </c>
       <c r="R1" s="34" t="s">
+        <v>236</v>
+      </c>
+      <c r="S1" s="34" t="s">
         <v>237</v>
       </c>
-      <c r="S1" s="34" t="s">
+      <c r="T1" s="10" t="s">
         <v>238</v>
-      </c>
-      <c r="T1" s="10" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
@@ -1360,19 +1364,19 @@
         <v>2</v>
       </c>
       <c r="B2" s="35" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C2" s="35" t="s">
         <v>18</v>
       </c>
       <c r="D2" s="36" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E2" s="35" t="s">
         <v>19</v>
       </c>
       <c r="F2" s="36" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="G2" s="35" t="s">
         <v>128</v>
@@ -1396,40 +1400,40 @@
         <v>3</v>
       </c>
       <c r="B3" s="35" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C3" s="35" t="s">
         <v>18</v>
       </c>
       <c r="D3" s="36" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E3" s="35" t="s">
         <v>19</v>
       </c>
       <c r="F3" s="36" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="G3" s="35" t="s">
         <v>128</v>
       </c>
       <c r="H3" s="35" t="s">
+        <v>179</v>
+      </c>
+      <c r="I3" s="35" t="s">
         <v>180</v>
       </c>
-      <c r="I3" s="35" t="s">
+      <c r="J3" s="35" t="s">
         <v>181</v>
       </c>
-      <c r="J3" s="35" t="s">
+      <c r="K3" s="35" t="s">
         <v>182</v>
       </c>
-      <c r="K3" s="35" t="s">
+      <c r="L3" s="35" t="s">
+        <v>182</v>
+      </c>
+      <c r="M3" s="35" t="s">
         <v>183</v>
-      </c>
-      <c r="L3" s="35" t="s">
-        <v>183</v>
-      </c>
-      <c r="M3" s="35" t="s">
-        <v>184</v>
       </c>
       <c r="N3" s="35"/>
       <c r="O3" s="35"/>
@@ -1444,19 +1448,19 @@
         <v>4</v>
       </c>
       <c r="B4" s="35" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C4" s="35" t="s">
         <v>18</v>
       </c>
       <c r="D4" s="36" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E4" s="35" t="s">
         <v>19</v>
       </c>
       <c r="F4" s="36" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="G4" s="35" t="s">
         <v>128</v>
@@ -1488,19 +1492,19 @@
         <v>5</v>
       </c>
       <c r="B5" s="35" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C5" s="35" t="s">
         <v>18</v>
       </c>
       <c r="D5" s="36" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E5" s="35" t="s">
         <v>19</v>
       </c>
       <c r="F5" s="36" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="G5" s="35" t="s">
         <v>128</v>
@@ -1524,19 +1528,19 @@
         <v>6</v>
       </c>
       <c r="B6" s="35" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C6" s="35" t="s">
         <v>18</v>
       </c>
       <c r="D6" s="36" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E6" s="35" t="s">
         <v>19</v>
       </c>
       <c r="F6" s="36" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="G6" s="35" t="s">
         <v>128</v>
@@ -1563,19 +1567,19 @@
         <v>7</v>
       </c>
       <c r="B7" s="35" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C7" s="35" t="s">
         <v>18</v>
       </c>
       <c r="D7" s="36" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E7" s="35" t="s">
         <v>19</v>
       </c>
       <c r="F7" s="36" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="G7" s="35" t="s">
         <v>128</v>
@@ -1601,19 +1605,19 @@
         <v>10</v>
       </c>
       <c r="B8" s="35" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C8" s="35" t="s">
         <v>18</v>
       </c>
       <c r="D8" s="36" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E8" s="35" t="s">
         <v>19</v>
       </c>
       <c r="F8" s="36" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="G8" s="35" t="s">
         <v>128</v>
@@ -1637,19 +1641,19 @@
         <v>11</v>
       </c>
       <c r="B9" s="35" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C9" s="35" t="s">
         <v>18</v>
       </c>
       <c r="D9" s="36" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E9" s="35" t="s">
         <v>19</v>
       </c>
       <c r="F9" s="36" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="G9" s="35" t="s">
         <v>128</v>
@@ -1968,34 +1972,34 @@
         <v>18</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" s="4" t="s">
         <v>187</v>
       </c>
-      <c r="E2" s="4" t="s">
-        <v>185</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G2" s="4" t="s">
+      <c r="H2" s="4" t="s">
         <v>188</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="I2" s="4" t="s">
         <v>189</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="J2" s="4" t="s">
         <v>190</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="K2" s="18" t="s">
         <v>191</v>
       </c>
-      <c r="K2" s="18" t="s">
+      <c r="L2" s="4" t="s">
         <v>192</v>
       </c>
-      <c r="L2" s="4" t="s">
+      <c r="M2" s="4" t="s">
         <v>193</v>
-      </c>
-      <c r="M2" s="4" t="s">
-        <v>194</v>
       </c>
       <c r="T2" s="2"/>
       <c r="U2" s="2"/>
@@ -2055,10 +2059,10 @@
         <v>18</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>19</v>
@@ -2071,22 +2075,22 @@
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
       <c r="N3" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="O3" s="5" t="s">
         <v>36</v>
       </c>
       <c r="P3" s="19" t="s">
+        <v>194</v>
+      </c>
+      <c r="Q3" s="19" t="s">
         <v>195</v>
-      </c>
-      <c r="Q3" s="19" t="s">
-        <v>196</v>
       </c>
       <c r="R3" s="19" t="s">
         <v>41</v>
       </c>
       <c r="S3" s="19" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="T3" s="2"/>
       <c r="U3" s="2"/>
@@ -2146,10 +2150,10 @@
         <v>18</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>19</v>
@@ -2168,25 +2172,25 @@
       <c r="R4" s="2"/>
       <c r="S4" s="2"/>
       <c r="T4" s="4" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="U4" s="4" t="s">
         <v>114</v>
       </c>
       <c r="V4" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="W4" s="4" t="s">
         <v>198</v>
       </c>
-      <c r="W4" s="4" t="s">
+      <c r="X4" s="4" t="s">
         <v>199</v>
       </c>
-      <c r="X4" s="4" t="s">
+      <c r="Y4" s="4" t="s">
         <v>200</v>
       </c>
-      <c r="Y4" s="4" t="s">
+      <c r="Z4" s="4" t="s">
         <v>201</v>
-      </c>
-      <c r="Z4" s="4" t="s">
-        <v>202</v>
       </c>
       <c r="AA4" s="2"/>
       <c r="AB4" s="2"/>
@@ -2239,10 +2243,10 @@
         <v>18</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>19</v>
@@ -2268,7 +2272,7 @@
       <c r="Y5" s="2"/>
       <c r="Z5" s="2"/>
       <c r="AA5" s="4" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="AB5" s="4" t="s">
         <v>49</v>
@@ -2277,19 +2281,19 @@
         <v>50</v>
       </c>
       <c r="AD5" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="AE5" s="4" t="s">
         <v>204</v>
       </c>
-      <c r="AE5" s="4" t="s">
+      <c r="AF5" s="36" t="s">
+        <v>240</v>
+      </c>
+      <c r="AG5" s="4" t="s">
         <v>205</v>
       </c>
-      <c r="AF5" s="36" t="s">
-        <v>241</v>
-      </c>
-      <c r="AG5" s="4" t="s">
+      <c r="AH5" s="4" t="s">
         <v>206</v>
-      </c>
-      <c r="AH5" s="4" t="s">
-        <v>207</v>
       </c>
       <c r="AI5" s="2"/>
       <c r="AJ5" s="2"/>
@@ -2334,10 +2338,10 @@
         <v>18</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>19</v>
@@ -2431,10 +2435,10 @@
         <v>18</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>19</v>
@@ -2526,10 +2530,10 @@
         <v>18</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>19</v>
@@ -2580,7 +2584,7 @@
       <c r="AX8" s="2"/>
       <c r="AY8" s="2"/>
       <c r="AZ8" s="17" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="BA8" s="2"/>
       <c r="BB8" s="2"/>
@@ -2607,10 +2611,10 @@
         <v>18</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>19</v>
@@ -2662,7 +2666,7 @@
       <c r="AY9" s="2"/>
       <c r="AZ9" s="2"/>
       <c r="BA9" s="4" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="BB9" s="2"/>
       <c r="BC9" s="2"/>
@@ -2688,10 +2692,10 @@
         <v>18</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>19</v>
@@ -2744,7 +2748,7 @@
       <c r="AZ10" s="2"/>
       <c r="BA10" s="2"/>
       <c r="BB10" s="4" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="BC10" s="2"/>
       <c r="BD10" s="2"/>
@@ -2769,10 +2773,10 @@
         <v>18</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>19</v>
@@ -2826,7 +2830,7 @@
       <c r="BA11" s="2"/>
       <c r="BB11" s="2"/>
       <c r="BC11" s="4" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="BD11" s="2"/>
       <c r="BE11" s="2"/>
@@ -2850,10 +2854,10 @@
         <v>18</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>19</v>
@@ -2908,7 +2912,7 @@
       <c r="BB12" s="2"/>
       <c r="BC12" s="2"/>
       <c r="BD12" s="4" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="BE12" s="2"/>
       <c r="BF12" s="2"/>
@@ -2931,10 +2935,10 @@
         <v>18</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>19</v>
@@ -3014,10 +3018,10 @@
         <v>18</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>19</v>
@@ -3095,10 +3099,10 @@
         <v>18</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>19</v>
@@ -3178,10 +3182,10 @@
         <v>18</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>19</v>
@@ -3261,10 +3265,10 @@
         <v>18</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F17" s="2" t="s">
         <v>19</v>
@@ -3400,11 +3404,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:L10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I4" sqref="I4"/>
+      <selection pane="bottomRight" activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3473,10 +3477,10 @@
         <v>18</v>
       </c>
       <c r="D2" s="22" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E2" s="23" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F2" s="22" t="s">
         <v>19</v>
@@ -3507,10 +3511,10 @@
         <v>18</v>
       </c>
       <c r="D3" s="22" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E3" s="23" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F3" s="22" t="s">
         <v>19</v>
@@ -3533,19 +3537,19 @@
         <v>18</v>
       </c>
       <c r="D4" s="22" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E4" s="23" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F4" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="G4" s="36" t="s">
-        <v>179</v>
+      <c r="G4" s="37" t="s">
+        <v>241</v>
       </c>
       <c r="H4" s="22" t="s">
-        <v>128</v>
+        <v>242</v>
       </c>
       <c r="I4" s="22"/>
       <c r="J4" s="22"/>
@@ -3563,10 +3567,10 @@
         <v>18</v>
       </c>
       <c r="D5" s="22" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E5" s="23" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F5" s="22" t="s">
         <v>19</v>
@@ -3589,10 +3593,10 @@
         <v>18</v>
       </c>
       <c r="D6" s="22" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E6" s="23" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F6" s="22" t="s">
         <v>19</v>
@@ -3615,10 +3619,10 @@
         <v>18</v>
       </c>
       <c r="D7" s="22" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E7" s="23" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F7" s="22" t="s">
         <v>19</v>
@@ -3641,10 +3645,10 @@
         <v>18</v>
       </c>
       <c r="D8" s="22" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E8" s="23" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F8" s="22" t="s">
         <v>19</v>
@@ -3667,10 +3671,10 @@
         <v>18</v>
       </c>
       <c r="D9" s="22" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E9" s="23" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F9" s="22" t="s">
         <v>19</v>
@@ -3693,10 +3697,10 @@
         <v>18</v>
       </c>
       <c r="D10" s="22" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E10" s="23" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F10" s="22" t="s">
         <v>19</v>
@@ -3713,7 +3717,7 @@
     <hyperlink ref="E3:E9" r:id="rId1" display="https://qat01.frontier.com/" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
     <hyperlink ref="E2" r:id="rId2" display="https://qat01.frontier.com/" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
     <hyperlink ref="E10" r:id="rId3" display="https://qat01.frontier.com/" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
-    <hyperlink ref="G4" r:id="rId4" xr:uid="{00000000-0004-0000-0200-000003000000}"/>
+    <hyperlink ref="G4" r:id="rId4" xr:uid="{946D5336-440C-4D1B-840F-DADDD6F71085}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId5"/>
@@ -3724,11 +3728,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:S17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G15" sqref="G15"/>
+      <selection pane="bottomRight" activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3825,16 +3829,16 @@
         <v>18</v>
       </c>
       <c r="D2" s="28" t="s">
+        <v>186</v>
+      </c>
+      <c r="E2" s="36" t="s">
+        <v>184</v>
+      </c>
+      <c r="F2" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" s="29" t="s">
         <v>187</v>
-      </c>
-      <c r="E2" s="29" t="s">
-        <v>185</v>
-      </c>
-      <c r="F2" s="28" t="s">
-        <v>19</v>
-      </c>
-      <c r="G2" s="29" t="s">
-        <v>188</v>
       </c>
       <c r="H2" s="29"/>
       <c r="I2" s="29"/>
@@ -3848,23 +3852,23 @@
         <v>2</v>
       </c>
       <c r="B3" s="35" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C3" s="28" t="s">
         <v>18</v>
       </c>
       <c r="D3" s="28" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E3" s="29" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F3" s="28" t="s">
         <v>19</v>
       </c>
       <c r="G3" s="28"/>
       <c r="H3" s="4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="I3" s="28"/>
       <c r="J3" s="28"/>
@@ -3883,16 +3887,16 @@
         <v>3</v>
       </c>
       <c r="B4" s="35" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C4" s="28" t="s">
         <v>18</v>
       </c>
       <c r="D4" s="28" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F4" s="28" t="s">
         <v>19</v>
@@ -3900,7 +3904,7 @@
       <c r="G4" s="28"/>
       <c r="H4" s="28"/>
       <c r="I4" s="4" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="J4" s="28"/>
       <c r="K4" s="28"/>
@@ -3918,16 +3922,16 @@
         <v>4</v>
       </c>
       <c r="B5" s="35" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C5" s="28" t="s">
         <v>18</v>
       </c>
       <c r="D5" s="28" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E5" s="29" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F5" s="28" t="s">
         <v>19</v>
@@ -3936,7 +3940,7 @@
       <c r="H5" s="28"/>
       <c r="I5" s="28"/>
       <c r="J5" s="5" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="K5" s="28"/>
       <c r="L5" s="28"/>
@@ -3953,16 +3957,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="35" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C6" s="28" t="s">
         <v>18</v>
       </c>
       <c r="D6" s="28" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E6" s="29" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F6" s="28" t="s">
         <v>19</v>
@@ -3972,7 +3976,7 @@
       <c r="I6" s="28"/>
       <c r="J6" s="28"/>
       <c r="K6" s="36" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="L6" s="28"/>
       <c r="M6" s="28"/>
@@ -3988,16 +3992,16 @@
         <v>6</v>
       </c>
       <c r="B7" s="35" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C7" s="28" t="s">
         <v>18</v>
       </c>
       <c r="D7" s="28" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E7" s="29" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F7" s="28" t="s">
         <v>19</v>
@@ -4008,7 +4012,7 @@
       <c r="J7" s="28"/>
       <c r="K7" s="28"/>
       <c r="L7" s="4" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="M7" s="28"/>
       <c r="N7" s="28"/>
@@ -4023,16 +4027,16 @@
         <v>7</v>
       </c>
       <c r="B8" s="35" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C8" s="28" t="s">
         <v>18</v>
       </c>
       <c r="D8" s="28" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E8" s="29" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F8" s="28" t="s">
         <v>19</v>
@@ -4056,16 +4060,16 @@
         <v>8</v>
       </c>
       <c r="B9" s="35" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C9" s="28" t="s">
         <v>18</v>
       </c>
       <c r="D9" s="28" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E9" s="29" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F9" s="28" t="s">
         <v>19</v>
@@ -4089,16 +4093,16 @@
         <v>9</v>
       </c>
       <c r="B10" s="35" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C10" s="28" t="s">
         <v>18</v>
       </c>
       <c r="D10" s="28" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E10" s="29" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F10" s="28" t="s">
         <v>19</v>
@@ -4122,16 +4126,16 @@
         <v>10</v>
       </c>
       <c r="B11" s="35" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C11" s="28" t="s">
         <v>18</v>
       </c>
       <c r="D11" s="28" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E11" s="29" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F11" s="28" t="s">
         <v>19</v>
@@ -4143,7 +4147,7 @@
       <c r="K11" s="28"/>
       <c r="L11" s="28"/>
       <c r="M11" s="4" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="N11" s="28"/>
       <c r="O11" s="28"/>
@@ -4157,16 +4161,16 @@
         <v>11</v>
       </c>
       <c r="B12" s="28" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C12" s="28" t="s">
         <v>18</v>
       </c>
       <c r="D12" s="28" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E12" s="29" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F12" s="28" t="s">
         <v>19</v>
@@ -4192,16 +4196,16 @@
         <v>12</v>
       </c>
       <c r="B13" s="28" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C13" s="28" t="s">
         <v>18</v>
       </c>
       <c r="D13" s="28" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E13" s="29" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F13" s="28" t="s">
         <v>19</v>
@@ -4215,7 +4219,7 @@
       <c r="M13" s="28"/>
       <c r="N13" s="28"/>
       <c r="O13" s="19" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="P13" s="28"/>
       <c r="Q13" s="28"/>
@@ -4227,16 +4231,16 @@
         <v>13</v>
       </c>
       <c r="B14" s="28" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C14" s="28" t="s">
         <v>18</v>
       </c>
       <c r="D14" s="28" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E14" s="29" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F14" s="28" t="s">
         <v>19</v>
@@ -4251,7 +4255,7 @@
       <c r="N14" s="28"/>
       <c r="O14" s="28"/>
       <c r="P14" s="4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="Q14" s="28"/>
       <c r="R14" s="28"/>
@@ -4262,16 +4266,16 @@
         <v>14</v>
       </c>
       <c r="B15" s="28" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C15" s="28" t="s">
         <v>18</v>
       </c>
       <c r="D15" s="28" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E15" s="29" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F15" s="28" t="s">
         <v>19</v>
@@ -4287,7 +4291,7 @@
       <c r="O15" s="28"/>
       <c r="P15" s="28"/>
       <c r="Q15" s="4" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="R15" s="28"/>
       <c r="S15" s="28"/>
@@ -4297,16 +4301,16 @@
         <v>15</v>
       </c>
       <c r="B16" s="28" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C16" s="28" t="s">
         <v>18</v>
       </c>
       <c r="D16" s="28" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E16" s="29" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F16" s="28" t="s">
         <v>19</v>
@@ -4323,7 +4327,7 @@
       <c r="P16" s="28"/>
       <c r="Q16" s="28"/>
       <c r="R16" s="4" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="S16" s="28"/>
     </row>
@@ -4332,16 +4336,16 @@
         <v>16</v>
       </c>
       <c r="B17" s="28" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C17" s="28" t="s">
         <v>18</v>
       </c>
       <c r="D17" s="28" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E17" s="29" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F17" s="28" t="s">
         <v>19</v>
@@ -4359,14 +4363,14 @@
       <c r="Q17" s="28"/>
       <c r="R17" s="28"/>
       <c r="S17" s="4" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E3:E16" r:id="rId1" display="https://qat01.frontier.com/" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
     <hyperlink ref="E17" r:id="rId2" display="https://qat01.frontier.com/" xr:uid="{00000000-0004-0000-0300-000001000000}"/>
-    <hyperlink ref="E2" r:id="rId3" display="https://qat01.frontier.com/" xr:uid="{00000000-0004-0000-0300-000002000000}"/>
+    <hyperlink ref="E2" r:id="rId3" xr:uid="{00000000-0004-0000-0300-000002000000}"/>
     <hyperlink ref="G2" r:id="rId4" display="https://qat01.frontier.com/shop/bundles" xr:uid="{00000000-0004-0000-0300-000003000000}"/>
     <hyperlink ref="H3" r:id="rId5" display="https://qat01.frontier.com/shop/internet" xr:uid="{00000000-0004-0000-0300-000004000000}"/>
     <hyperlink ref="I4" r:id="rId6" display="https://qat01.frontier.com/shop/phone" xr:uid="{00000000-0004-0000-0300-000005000000}"/>

</xml_diff>

<commit_message>
added ECOMM test cases
</commit_message>
<xml_diff>
--- a/Resources/TestData/qat03.xlsx
+++ b/Resources/TestData/qat03.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18625"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="517" uniqueCount="248">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="524" uniqueCount="250">
   <si>
     <t>TC_NO</t>
   </si>
@@ -772,6 +772,12 @@
   </si>
   <si>
     <t>3800</t>
+  </si>
+  <si>
+    <t>HopUpdrage</t>
+  </si>
+  <si>
+    <t>Ftrfrank1+ecomauto@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -1286,13 +1292,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T9"/>
+  <dimension ref="A1:T10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="S6" sqref="S6"/>
+      <selection pane="bottomRight" activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1695,14 +1701,53 @@
       <c r="S9" s="35"/>
       <c r="T9" s="35"/>
     </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A10" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="35" t="s">
+        <v>248</v>
+      </c>
+      <c r="C10" s="35" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="36" t="s">
+        <v>184</v>
+      </c>
+      <c r="E10" s="35" t="s">
+        <v>19</v>
+      </c>
+      <c r="F10" s="36" t="s">
+        <v>249</v>
+      </c>
+      <c r="G10" s="35" t="s">
+        <v>128</v>
+      </c>
+      <c r="H10" s="35"/>
+      <c r="I10" s="35"/>
+      <c r="J10" s="35"/>
+      <c r="K10" s="35"/>
+      <c r="L10" s="35"/>
+      <c r="M10" s="35"/>
+      <c r="N10" s="35"/>
+      <c r="O10" s="35"/>
+      <c r="P10" s="35"/>
+      <c r="Q10" s="35"/>
+      <c r="R10" s="35"/>
+      <c r="S10" s="35"/>
+      <c r="T10" s="35"/>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D9" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
     <hyperlink ref="F2" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="D2" r:id="rId3" display="https://qat01.frontier.com/" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="D2" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="D6" r:id="rId4" xr:uid="{069EBF77-4D15-4A56-96A2-FA48CB1466A3}"/>
+    <hyperlink ref="D10" r:id="rId5" xr:uid="{428E0D5F-5715-4602-9AB0-50B80738155C}"/>
+    <hyperlink ref="F10" r:id="rId6" xr:uid="{7AC2C3E6-C4D6-4DED-B452-E98FDEA12325}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId4"/>
+  <pageSetup orientation="portrait" r:id="rId7"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Modified Chat test cases
</commit_message>
<xml_diff>
--- a/Resources/TestData/qat03.xlsx
+++ b/Resources/TestData/qat03.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19330"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\Robot\DotCom\Resources\TestData\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D735C66-1A95-4B0B-A375-9554CDCA18A1}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25440" windowHeight="12210" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25440" windowHeight="12210" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="REG" sheetId="4" r:id="rId1"/>
@@ -26,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="982" uniqueCount="299">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="982" uniqueCount="297">
   <si>
     <t>TC_NO</t>
   </si>
@@ -600,12 +606,6 @@
     <t>Chrome</t>
   </si>
   <si>
-    <t>https://qat02.frontier.com/</t>
-  </si>
-  <si>
-    <t>https://qat02.frontier.com/resources/cpni</t>
-  </si>
-  <si>
     <t>009_CC_.COM_NSS_Res_Multi-Language_OnlineAndMobile_SiteWideTranslationNavigation</t>
   </si>
   <si>
@@ -975,7 +975,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1469,14 +1469,14 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1577,7 +1577,7 @@
         <v>18</v>
       </c>
       <c r="F2" s="27" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="G2" s="26" t="s">
         <v>99</v>
@@ -1647,7 +1647,7 @@
         <v>18</v>
       </c>
       <c r="F4" s="27" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="G4" s="26" t="s">
         <v>99</v>
@@ -1688,7 +1688,7 @@
         <v>18</v>
       </c>
       <c r="F5" s="27" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="G5" s="26" t="s">
         <v>99</v>
@@ -1721,7 +1721,7 @@
         <v>18</v>
       </c>
       <c r="F6" s="27" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="G6" s="26" t="s">
         <v>99</v>
@@ -1758,7 +1758,7 @@
         <v>18</v>
       </c>
       <c r="F7" s="27" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="G7" s="26" t="s">
         <v>99</v>
@@ -1793,7 +1793,7 @@
         <v>18</v>
       </c>
       <c r="F8" s="27" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="G8" s="26" t="s">
         <v>99</v>
@@ -1820,13 +1820,13 @@
         <v>174</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="E9" s="26" t="s">
         <v>18</v>
       </c>
       <c r="F9" s="27" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="G9" s="26" t="s">
         <v>99</v>
@@ -1859,13 +1859,13 @@
         <v>18</v>
       </c>
       <c r="F10" s="27" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="G10" s="26" t="s">
         <v>99</v>
       </c>
       <c r="H10" s="32" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="I10" s="26"/>
       <c r="J10" s="26"/>
@@ -1896,7 +1896,7 @@
         <v>18</v>
       </c>
       <c r="F11" s="27" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="G11" s="26" t="s">
         <v>99</v>
@@ -1933,25 +1933,25 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1"/>
-    <hyperlink ref="F11" r:id="rId2"/>
-    <hyperlink ref="F6" r:id="rId3"/>
-    <hyperlink ref="F7" r:id="rId4"/>
-    <hyperlink ref="F4" r:id="rId5"/>
-    <hyperlink ref="F5" r:id="rId6"/>
-    <hyperlink ref="F10" r:id="rId7"/>
-    <hyperlink ref="D2" r:id="rId8"/>
-    <hyperlink ref="D9" r:id="rId9"/>
-    <hyperlink ref="D10" r:id="rId10"/>
-    <hyperlink ref="D11" r:id="rId11"/>
-    <hyperlink ref="D3" r:id="rId12"/>
-    <hyperlink ref="D4" r:id="rId13"/>
-    <hyperlink ref="D5" r:id="rId14"/>
-    <hyperlink ref="D6" r:id="rId15"/>
-    <hyperlink ref="D7" r:id="rId16"/>
-    <hyperlink ref="D8" r:id="rId17"/>
-    <hyperlink ref="F8" r:id="rId18"/>
-    <hyperlink ref="F9" r:id="rId19"/>
+    <hyperlink ref="F2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="F11" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="F6" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="F7" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="F4" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="F5" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="F10" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="D2" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="D9" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="D10" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="D11" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="D3" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="D4" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="D5" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="D6" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="D7" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="D8" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="F8" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="F9" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId20"/>
@@ -1959,10 +1959,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:O42"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E42" sqref="E42"/>
     </sheetView>
   </sheetViews>
@@ -2028,7 +2028,7 @@
         <v>174</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>175</v>
+        <v>69</v>
       </c>
       <c r="E2" s="8" t="s">
         <v>18</v>
@@ -2059,7 +2059,7 @@
         <v>174</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>175</v>
+        <v>69</v>
       </c>
       <c r="E3" s="8" t="s">
         <v>18</v>
@@ -2086,7 +2086,7 @@
         <v>174</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>175</v>
+        <v>69</v>
       </c>
       <c r="E4" s="8" t="s">
         <v>18</v>
@@ -2113,7 +2113,7 @@
         <v>174</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>175</v>
+        <v>69</v>
       </c>
       <c r="E5" s="8" t="s">
         <v>18</v>
@@ -2138,7 +2138,7 @@
         <v>174</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>175</v>
+        <v>69</v>
       </c>
       <c r="E6" s="8" t="s">
         <v>18</v>
@@ -2165,7 +2165,7 @@
         <v>174</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>175</v>
+        <v>69</v>
       </c>
       <c r="E7" s="8" t="s">
         <v>18</v>
@@ -2192,7 +2192,7 @@
         <v>174</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>175</v>
+        <v>69</v>
       </c>
       <c r="E8" s="8" t="s">
         <v>18</v>
@@ -2219,7 +2219,7 @@
         <v>174</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>176</v>
+        <v>290</v>
       </c>
       <c r="E9" s="8" t="s">
         <v>18</v>
@@ -2240,13 +2240,13 @@
         <v>9</v>
       </c>
       <c r="B10" s="36" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C10" s="37" t="s">
         <v>174</v>
       </c>
       <c r="D10" s="38" t="s">
-        <v>175</v>
+        <v>69</v>
       </c>
       <c r="E10" s="37" t="s">
         <v>18</v>
@@ -2273,7 +2273,7 @@
         <v>174</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>175</v>
+        <v>69</v>
       </c>
       <c r="E11" s="8" t="s">
         <v>18</v>
@@ -2300,7 +2300,7 @@
         <v>174</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>175</v>
+        <v>69</v>
       </c>
       <c r="E12" s="8" t="s">
         <v>18</v>
@@ -2327,7 +2327,7 @@
         <v>174</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>175</v>
+        <v>69</v>
       </c>
       <c r="E13" s="8" t="s">
         <v>18</v>
@@ -2354,7 +2354,7 @@
         <v>174</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>175</v>
+        <v>69</v>
       </c>
       <c r="E14" s="8" t="s">
         <v>18</v>
@@ -2381,7 +2381,7 @@
         <v>174</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>175</v>
+        <v>69</v>
       </c>
       <c r="E15" s="8" t="s">
         <v>18</v>
@@ -2408,7 +2408,7 @@
         <v>174</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>175</v>
+        <v>69</v>
       </c>
       <c r="E16" s="8" t="s">
         <v>18</v>
@@ -2435,7 +2435,7 @@
         <v>174</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>175</v>
+        <v>69</v>
       </c>
       <c r="E17" s="8" t="s">
         <v>18</v>
@@ -2462,7 +2462,7 @@
         <v>174</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>175</v>
+        <v>69</v>
       </c>
       <c r="E18" s="8" t="s">
         <v>18</v>
@@ -3045,7 +3045,7 @@
         <v>174</v>
       </c>
       <c r="D40" s="27" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="E40" s="8"/>
       <c r="F40" s="8"/>
@@ -3070,7 +3070,7 @@
         <v>174</v>
       </c>
       <c r="D41" s="27" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="E41" s="8"/>
       <c r="F41" s="8"/>
@@ -3095,7 +3095,7 @@
         <v>174</v>
       </c>
       <c r="D42" s="27" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="E42" s="8"/>
       <c r="F42" s="8"/>
@@ -3111,35 +3111,35 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D9" r:id="rId1" display="https://qat03.frontier.com/resources/cpni"/>
-    <hyperlink ref="F2" r:id="rId2"/>
-    <hyperlink ref="D2" r:id="rId3" display="https://qat03.frontier.com/"/>
-    <hyperlink ref="D6" r:id="rId4" display="https://qat03.frontier.com/"/>
-    <hyperlink ref="D10" r:id="rId5" display="https://qat03.frontier.com/"/>
-    <hyperlink ref="D11" r:id="rId6" display="https://qat03.frontier.com/"/>
-    <hyperlink ref="D12" r:id="rId7" display="https://qat03.frontier.com/"/>
-    <hyperlink ref="D13" r:id="rId8" display="https://qat03.frontier.com/"/>
-    <hyperlink ref="D14" r:id="rId9" display="https://qat03.frontier.com/"/>
-    <hyperlink ref="D15" r:id="rId10" display="https://qat03.frontier.com/"/>
-    <hyperlink ref="D16" r:id="rId11" display="https://qat03.frontier.com/"/>
-    <hyperlink ref="D17" r:id="rId12" display="https://qat03.frontier.com/"/>
-    <hyperlink ref="D18" r:id="rId13" display="https://qat03.frontier.com/"/>
-    <hyperlink ref="D19" r:id="rId14"/>
-    <hyperlink ref="D25" r:id="rId15"/>
-    <hyperlink ref="D27" r:id="rId16"/>
-    <hyperlink ref="D28" r:id="rId17"/>
-    <hyperlink ref="D29" r:id="rId18"/>
-    <hyperlink ref="D30" r:id="rId19"/>
-    <hyperlink ref="D41" r:id="rId20" location="/"/>
-    <hyperlink ref="D42" r:id="rId21" location="/"/>
-    <hyperlink ref="D40" r:id="rId22" location="/"/>
+    <hyperlink ref="D9" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="F2" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="D2" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
+    <hyperlink ref="D6" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
+    <hyperlink ref="D10" r:id="rId5" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
+    <hyperlink ref="D11" r:id="rId6" xr:uid="{00000000-0004-0000-0100-000005000000}"/>
+    <hyperlink ref="D12" r:id="rId7" xr:uid="{00000000-0004-0000-0100-000006000000}"/>
+    <hyperlink ref="D13" r:id="rId8" xr:uid="{00000000-0004-0000-0100-000007000000}"/>
+    <hyperlink ref="D14" r:id="rId9" xr:uid="{00000000-0004-0000-0100-000008000000}"/>
+    <hyperlink ref="D15" r:id="rId10" xr:uid="{00000000-0004-0000-0100-000009000000}"/>
+    <hyperlink ref="D16" r:id="rId11" xr:uid="{00000000-0004-0000-0100-00000A000000}"/>
+    <hyperlink ref="D17" r:id="rId12" xr:uid="{00000000-0004-0000-0100-00000B000000}"/>
+    <hyperlink ref="D18" r:id="rId13" xr:uid="{00000000-0004-0000-0100-00000C000000}"/>
+    <hyperlink ref="D19" r:id="rId14" xr:uid="{00000000-0004-0000-0100-00000D000000}"/>
+    <hyperlink ref="D25" r:id="rId15" xr:uid="{00000000-0004-0000-0100-00000E000000}"/>
+    <hyperlink ref="D27" r:id="rId16" xr:uid="{00000000-0004-0000-0100-00000F000000}"/>
+    <hyperlink ref="D28" r:id="rId17" xr:uid="{00000000-0004-0000-0100-000010000000}"/>
+    <hyperlink ref="D29" r:id="rId18" xr:uid="{00000000-0004-0000-0100-000011000000}"/>
+    <hyperlink ref="D30" r:id="rId19" xr:uid="{00000000-0004-0000-0100-000012000000}"/>
+    <hyperlink ref="D41" r:id="rId20" location="/" xr:uid="{00000000-0004-0000-0100-000013000000}"/>
+    <hyperlink ref="D42" r:id="rId21" location="/" xr:uid="{00000000-0004-0000-0100-000014000000}"/>
+    <hyperlink ref="D40" r:id="rId22" location="/" xr:uid="{00000000-0004-0000-0100-000015000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3502,9 +3502,9 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E3:E16" r:id="rId1" display="https://qat01.frontier.com/"/>
-    <hyperlink ref="E17" r:id="rId2" display="https://qat01.frontier.com/"/>
-    <hyperlink ref="E2" r:id="rId3"/>
+    <hyperlink ref="E3:E16" r:id="rId1" display="https://qat01.frontier.com/" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="E17" r:id="rId2" display="https://qat01.frontier.com/" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
+    <hyperlink ref="E2" r:id="rId3" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId4"/>
@@ -3512,7 +3512,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:L10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3825,10 +3825,10 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E3:E9" r:id="rId1" display="https://qat01.frontier.com/"/>
-    <hyperlink ref="E2" r:id="rId2" display="https://qat01.frontier.com/"/>
-    <hyperlink ref="E10" r:id="rId3" display="https://qat01.frontier.com/"/>
-    <hyperlink ref="G4" r:id="rId4"/>
+    <hyperlink ref="E3:E9" r:id="rId1" display="https://qat01.frontier.com/" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
+    <hyperlink ref="E2" r:id="rId2" display="https://qat01.frontier.com/" xr:uid="{00000000-0004-0000-0300-000001000000}"/>
+    <hyperlink ref="E10" r:id="rId3" display="https://qat01.frontier.com/" xr:uid="{00000000-0004-0000-0300-000002000000}"/>
+    <hyperlink ref="G4" r:id="rId4" xr:uid="{00000000-0004-0000-0300-000003000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId5"/>
@@ -3836,7 +3836,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4147,9 +4147,9 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D3:D16" r:id="rId1" display="https://qat01.frontier.com/"/>
-    <hyperlink ref="D17" r:id="rId2" display="https://qat01.frontier.com/"/>
-    <hyperlink ref="D2" r:id="rId3"/>
+    <hyperlink ref="D3:D16" r:id="rId1" display="https://qat01.frontier.com/" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
+    <hyperlink ref="D17" r:id="rId2" display="https://qat01.frontier.com/" xr:uid="{00000000-0004-0000-0400-000001000000}"/>
+    <hyperlink ref="D2" r:id="rId3" xr:uid="{00000000-0004-0000-0400-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId4"/>
@@ -4157,7 +4157,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:O21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4245,7 +4245,7 @@
         <v>18</v>
       </c>
       <c r="F3" s="20" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="G3" s="27" t="s">
         <v>99</v>
@@ -4276,7 +4276,7 @@
         <v>18</v>
       </c>
       <c r="F4" s="20" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="G4" s="27" t="s">
         <v>99</v>
@@ -4307,7 +4307,7 @@
         <v>18</v>
       </c>
       <c r="F5" s="20" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="G5" s="27" t="s">
         <v>99</v>
@@ -4338,7 +4338,7 @@
         <v>18</v>
       </c>
       <c r="F6" s="20" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="G6" s="27" t="s">
         <v>99</v>
@@ -4369,7 +4369,7 @@
         <v>18</v>
       </c>
       <c r="F7" s="20" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="G7" s="27" t="s">
         <v>99</v>
@@ -4623,15 +4623,15 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D3" r:id="rId1"/>
-    <hyperlink ref="F3" r:id="rId2"/>
-    <hyperlink ref="D4" r:id="rId3"/>
-    <hyperlink ref="D5" r:id="rId4"/>
-    <hyperlink ref="F5" r:id="rId5"/>
-    <hyperlink ref="D6" r:id="rId6"/>
-    <hyperlink ref="F6" r:id="rId7"/>
-    <hyperlink ref="D7" r:id="rId8"/>
-    <hyperlink ref="F7" r:id="rId9"/>
+    <hyperlink ref="D3" r:id="rId1" xr:uid="{00000000-0004-0000-0500-000000000000}"/>
+    <hyperlink ref="F3" r:id="rId2" xr:uid="{00000000-0004-0000-0500-000001000000}"/>
+    <hyperlink ref="D4" r:id="rId3" xr:uid="{00000000-0004-0000-0500-000002000000}"/>
+    <hyperlink ref="D5" r:id="rId4" xr:uid="{00000000-0004-0000-0500-000003000000}"/>
+    <hyperlink ref="F5" r:id="rId5" xr:uid="{00000000-0004-0000-0500-000004000000}"/>
+    <hyperlink ref="D6" r:id="rId6" xr:uid="{00000000-0004-0000-0500-000005000000}"/>
+    <hyperlink ref="F6" r:id="rId7" xr:uid="{00000000-0004-0000-0500-000006000000}"/>
+    <hyperlink ref="D7" r:id="rId8" xr:uid="{00000000-0004-0000-0500-000007000000}"/>
+    <hyperlink ref="F7" r:id="rId9" xr:uid="{00000000-0004-0000-0500-000008000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId10"/>
@@ -4639,7 +4639,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4686,7 +4686,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C2" s="26" t="s">
         <v>174</v>
@@ -4705,7 +4705,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C3" s="26" t="s">
         <v>174</v>
@@ -4724,7 +4724,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C4" s="26" t="s">
         <v>174</v>
@@ -4743,7 +4743,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C5" s="26" t="s">
         <v>174</v>
@@ -4762,7 +4762,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C6" s="26" t="s">
         <v>174</v>
@@ -4781,7 +4781,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C7" s="26" t="s">
         <v>174</v>
@@ -4800,7 +4800,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C8" s="26" t="s">
         <v>174</v>
@@ -4819,7 +4819,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C9" s="26" t="s">
         <v>174</v>
@@ -4838,7 +4838,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C10" s="26" t="s">
         <v>174</v>
@@ -4858,7 +4858,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:K54"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
@@ -4885,7 +4885,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C1" s="6" t="s">
         <v>21</v>
@@ -4912,14 +4912,14 @@
         <v>55</v>
       </c>
       <c r="K1" s="6" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="40"/>
       <c r="B2" s="40"/>
       <c r="C2" s="40" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D2" s="40"/>
       <c r="E2" s="40"/>
@@ -4935,10 +4935,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D3" s="26" t="s">
         <v>174</v>
@@ -4962,10 +4962,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="8" t="s">
+        <v>187</v>
+      </c>
+      <c r="C4" s="8" t="s">
         <v>189</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>191</v>
       </c>
       <c r="D4" s="26" t="s">
         <v>174</v>
@@ -4989,10 +4989,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D5" s="26" t="s">
         <v>174</v>
@@ -5006,13 +5006,13 @@
       <c r="G5" s="20"/>
       <c r="H5" s="8"/>
       <c r="I5" s="26" t="s">
+        <v>191</v>
+      </c>
+      <c r="J5" s="26" t="s">
+        <v>192</v>
+      </c>
+      <c r="K5" s="26" t="s">
         <v>193</v>
-      </c>
-      <c r="J5" s="26" t="s">
-        <v>194</v>
-      </c>
-      <c r="K5" s="26" t="s">
-        <v>195</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -5020,10 +5020,10 @@
         <v>4</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="D6" s="26" t="s">
         <v>174</v>
@@ -5045,10 +5045,10 @@
         <v>5</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D7" s="26" t="s">
         <v>174</v>
@@ -5062,7 +5062,7 @@
       <c r="G7" s="8"/>
       <c r="H7" s="8"/>
       <c r="I7" s="26" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="J7" s="26"/>
       <c r="K7" s="26"/>
@@ -5072,10 +5072,10 @@
         <v>6</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="D8" s="26" t="s">
         <v>174</v>
@@ -5089,7 +5089,7 @@
       <c r="G8" s="8"/>
       <c r="H8" s="8"/>
       <c r="I8" s="26" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="J8" s="26"/>
       <c r="K8" s="26"/>
@@ -5099,10 +5099,10 @@
         <v>7</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D9" s="26" t="s">
         <v>174</v>
@@ -5116,7 +5116,7 @@
       <c r="G9" s="8"/>
       <c r="H9" s="8"/>
       <c r="I9" s="26" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="J9" s="26"/>
       <c r="K9" s="26"/>
@@ -5126,10 +5126,10 @@
         <v>8</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="D10" s="26" t="s">
         <v>174</v>
@@ -5143,7 +5143,7 @@
       <c r="G10" s="8"/>
       <c r="H10" s="8"/>
       <c r="I10" s="26" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="J10" s="26"/>
       <c r="K10" s="26"/>
@@ -5153,10 +5153,10 @@
         <v>9</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D11" s="26" t="s">
         <v>174</v>
@@ -5170,7 +5170,7 @@
       <c r="G11" s="8"/>
       <c r="H11" s="8"/>
       <c r="I11" s="26" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="J11" s="26"/>
       <c r="K11" s="26"/>
@@ -5179,7 +5179,7 @@
       <c r="A12" s="40"/>
       <c r="B12" s="40"/>
       <c r="C12" s="40" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D12" s="40"/>
       <c r="E12" s="40"/>
@@ -5192,13 +5192,13 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="42" t="s">
+        <v>206</v>
+      </c>
+      <c r="B13" s="43" t="s">
+        <v>207</v>
+      </c>
+      <c r="C13" s="44" t="s">
         <v>208</v>
-      </c>
-      <c r="B13" s="43" t="s">
-        <v>209</v>
-      </c>
-      <c r="C13" s="44" t="s">
-        <v>210</v>
       </c>
       <c r="D13" s="26"/>
       <c r="E13" s="9"/>
@@ -5211,13 +5211,13 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="42" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B14" s="43" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C14" s="24" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="D14" s="26" t="s">
         <v>174</v>
@@ -5231,20 +5231,20 @@
       <c r="G14" s="45"/>
       <c r="H14" s="45"/>
       <c r="I14" s="26" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="J14" s="26"/>
       <c r="K14" s="26"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="42" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B15" s="43" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C15" s="44" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D15" s="26"/>
       <c r="E15" s="9"/>
@@ -5257,13 +5257,13 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="42" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B16" s="43" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C16" s="24" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D16" s="26" t="s">
         <v>174</v>
@@ -5277,20 +5277,20 @@
       <c r="G16" s="45"/>
       <c r="H16" s="45"/>
       <c r="I16" s="26" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="J16" s="26"/>
       <c r="K16" s="26"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="42" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B17" s="43" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C17" s="24" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="D17" s="26" t="s">
         <v>174</v>
@@ -5304,20 +5304,20 @@
       <c r="G17" s="45"/>
       <c r="H17" s="45"/>
       <c r="I17" s="26" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="J17" s="26"/>
       <c r="K17" s="26"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="42" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B18" s="43" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C18" s="24" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D18" s="26" t="s">
         <v>174</v>
@@ -5331,20 +5331,20 @@
       <c r="G18" s="45"/>
       <c r="H18" s="45"/>
       <c r="I18" s="26" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="J18" s="26"/>
       <c r="K18" s="26"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="42" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B19" s="43" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C19" s="24" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="D19" s="26" t="s">
         <v>174</v>
@@ -5358,20 +5358,20 @@
       <c r="G19" s="45"/>
       <c r="H19" s="45"/>
       <c r="I19" s="26" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="J19" s="26"/>
       <c r="K19" s="26"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="42" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B20" s="43" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C20" s="44" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="D20" s="26"/>
       <c r="E20" s="9"/>
@@ -5384,13 +5384,13 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="42" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B21" s="43" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C21" s="24" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="D21" s="26" t="s">
         <v>174</v>
@@ -5404,20 +5404,20 @@
       <c r="G21" s="45"/>
       <c r="H21" s="45"/>
       <c r="I21" s="26" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="J21" s="26"/>
       <c r="K21" s="26"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="42" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B22" s="43" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C22" s="24" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="D22" s="26" t="s">
         <v>174</v>
@@ -5431,20 +5431,20 @@
       <c r="G22" s="45"/>
       <c r="H22" s="45"/>
       <c r="I22" s="26" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="J22" s="26"/>
       <c r="K22" s="26"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="42" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B23" s="43" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C23" s="24" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="D23" s="26" t="s">
         <v>174</v>
@@ -5458,20 +5458,20 @@
       <c r="G23" s="45"/>
       <c r="H23" s="45"/>
       <c r="I23" s="26" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="J23" s="26"/>
       <c r="K23" s="26"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="42" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B24" s="43" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C24" s="24" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="D24" s="26" t="s">
         <v>174</v>
@@ -5485,20 +5485,20 @@
       <c r="G24" s="45"/>
       <c r="H24" s="45"/>
       <c r="I24" s="26" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="J24" s="26"/>
       <c r="K24" s="26"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="42" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B25" s="43" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C25" s="24" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D25" s="26" t="s">
         <v>174</v>
@@ -5512,20 +5512,20 @@
       <c r="G25" s="45"/>
       <c r="H25" s="45"/>
       <c r="I25" s="26" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="J25" s="26"/>
       <c r="K25" s="26"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="42" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B26" s="43" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C26" s="44" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="D26" s="26"/>
       <c r="E26" s="9"/>
@@ -5538,13 +5538,13 @@
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="42" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B27" s="43" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C27" s="24" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="D27" s="26" t="s">
         <v>174</v>
@@ -5558,20 +5558,20 @@
       <c r="G27" s="45"/>
       <c r="H27" s="45"/>
       <c r="I27" s="26" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="J27" s="26"/>
       <c r="K27" s="26"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="42" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="B28" s="43" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C28" s="24" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="D28" s="26" t="s">
         <v>174</v>
@@ -5585,20 +5585,20 @@
       <c r="G28" s="45"/>
       <c r="H28" s="45"/>
       <c r="I28" s="26" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="J28" s="26"/>
       <c r="K28" s="26"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="42" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="B29" s="43" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C29" s="24" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="D29" s="26" t="s">
         <v>174</v>
@@ -5612,20 +5612,20 @@
       <c r="G29" s="45"/>
       <c r="H29" s="45"/>
       <c r="I29" s="26" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="J29" s="26"/>
       <c r="K29" s="26"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="42" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B30" s="43" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C30" s="24" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="D30" s="26" t="s">
         <v>174</v>
@@ -5639,20 +5639,20 @@
       <c r="G30" s="45"/>
       <c r="H30" s="45"/>
       <c r="I30" s="26" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="J30" s="26"/>
       <c r="K30" s="26"/>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="42" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="B31" s="43" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C31" s="24" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="D31" s="26" t="s">
         <v>174</v>
@@ -5666,20 +5666,20 @@
       <c r="G31" s="45"/>
       <c r="H31" s="45"/>
       <c r="I31" s="26" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="J31" s="26"/>
       <c r="K31" s="26"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="42" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="B32" s="43" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C32" s="24" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="D32" s="26" t="s">
         <v>174</v>
@@ -5693,20 +5693,20 @@
       <c r="G32" s="45"/>
       <c r="H32" s="45"/>
       <c r="I32" s="26" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="J32" s="26"/>
       <c r="K32" s="26"/>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="42" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="B33" s="43" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C33" s="24" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="D33" s="26" t="s">
         <v>174</v>
@@ -5720,20 +5720,20 @@
       <c r="G33" s="45"/>
       <c r="H33" s="45"/>
       <c r="I33" s="26" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="J33" s="26"/>
       <c r="K33" s="26"/>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="42" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="B34" s="43" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C34" s="24" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="D34" s="26" t="s">
         <v>174</v>
@@ -5747,20 +5747,20 @@
       <c r="G34" s="45"/>
       <c r="H34" s="45"/>
       <c r="I34" s="26" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="J34" s="26"/>
       <c r="K34" s="26"/>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="42" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B35" s="43" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C35" s="24" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="D35" s="26" t="s">
         <v>174</v>
@@ -5774,20 +5774,20 @@
       <c r="G35" s="45"/>
       <c r="H35" s="45"/>
       <c r="I35" s="26" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="J35" s="26"/>
       <c r="K35" s="26"/>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="42" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="B36" s="43" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C36" s="24" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="D36" s="26" t="s">
         <v>174</v>
@@ -5801,20 +5801,20 @@
       <c r="G36" s="45"/>
       <c r="H36" s="45"/>
       <c r="I36" s="26" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="J36" s="26"/>
       <c r="K36" s="26"/>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="42" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B37" s="43" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C37" s="24" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="D37" s="26" t="s">
         <v>174</v>
@@ -5828,7 +5828,7 @@
       <c r="G37" s="45"/>
       <c r="H37" s="45"/>
       <c r="I37" s="26" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="J37" s="26"/>
       <c r="K37" s="26"/>
@@ -5837,7 +5837,7 @@
       <c r="A38" s="40"/>
       <c r="B38" s="40"/>
       <c r="C38" s="40" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="D38" s="40"/>
       <c r="E38" s="40"/>
@@ -5853,10 +5853,10 @@
         <v>158</v>
       </c>
       <c r="B39" s="43" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C39" s="46" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="D39" s="14" t="s">
         <v>174</v>
@@ -5870,7 +5870,7 @@
       <c r="G39" s="46"/>
       <c r="H39" s="46"/>
       <c r="I39" s="16" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="J39" s="16"/>
       <c r="K39" s="16"/>
@@ -5880,10 +5880,10 @@
         <v>160</v>
       </c>
       <c r="B40" s="43" t="s">
+        <v>264</v>
+      </c>
+      <c r="C40" s="46" t="s">
         <v>266</v>
-      </c>
-      <c r="C40" s="46" t="s">
-        <v>268</v>
       </c>
       <c r="D40" s="14" t="s">
         <v>174</v>
@@ -5897,7 +5897,7 @@
       <c r="G40" s="46"/>
       <c r="H40" s="46"/>
       <c r="I40" s="26" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="J40" s="16"/>
       <c r="K40" s="16"/>
@@ -5907,10 +5907,10 @@
         <v>162</v>
       </c>
       <c r="B41" s="43" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C41" s="46" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="D41" s="14" t="s">
         <v>174</v>
@@ -5924,7 +5924,7 @@
       <c r="G41" s="46"/>
       <c r="H41" s="46"/>
       <c r="I41" s="16" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="J41" s="16"/>
       <c r="K41" s="16"/>
@@ -5934,10 +5934,10 @@
         <v>163</v>
       </c>
       <c r="B42" s="43" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C42" s="46" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="D42" s="14" t="s">
         <v>174</v>
@@ -5951,7 +5951,7 @@
       <c r="G42" s="46"/>
       <c r="H42" s="46"/>
       <c r="I42" s="14" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="J42" s="16"/>
       <c r="K42" s="16"/>
@@ -5961,10 +5961,10 @@
         <v>164</v>
       </c>
       <c r="B43" s="43" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C43" s="46" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="D43" s="14" t="s">
         <v>174</v>
@@ -5978,7 +5978,7 @@
       <c r="G43" s="46"/>
       <c r="H43" s="46"/>
       <c r="I43" s="14" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="J43" s="16"/>
       <c r="K43" s="16"/>
@@ -5988,10 +5988,10 @@
         <v>165</v>
       </c>
       <c r="B44" s="43" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C44" s="46" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="D44" s="14" t="s">
         <v>174</v>
@@ -6005,7 +6005,7 @@
       <c r="G44" s="46"/>
       <c r="H44" s="46"/>
       <c r="I44" s="14" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="J44" s="16"/>
       <c r="K44" s="16"/>
@@ -6015,10 +6015,10 @@
         <v>167</v>
       </c>
       <c r="B45" s="43" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="C45" s="46" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="D45" s="14" t="s">
         <v>174</v>
@@ -6032,7 +6032,7 @@
       <c r="G45" s="46"/>
       <c r="H45" s="46"/>
       <c r="I45" s="16" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="J45" s="16"/>
       <c r="K45" s="16"/>
@@ -6042,10 +6042,10 @@
         <v>169</v>
       </c>
       <c r="B46" s="43" t="s">
+        <v>272</v>
+      </c>
+      <c r="C46" s="46" t="s">
         <v>274</v>
-      </c>
-      <c r="C46" s="46" t="s">
-        <v>276</v>
       </c>
       <c r="D46" s="14" t="s">
         <v>174</v>
@@ -6059,20 +6059,20 @@
       <c r="G46" s="46"/>
       <c r="H46" s="46"/>
       <c r="I46" s="26" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="J46" s="16"/>
       <c r="K46" s="16"/>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" s="42" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B47" s="43" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="C47" s="46" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="D47" s="14" t="s">
         <v>174</v>
@@ -6086,20 +6086,20 @@
       <c r="G47" s="46"/>
       <c r="H47" s="46"/>
       <c r="I47" s="16" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="J47" s="16"/>
       <c r="K47" s="16"/>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" s="42" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B48" s="43" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="C48" s="46" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="D48" s="14" t="s">
         <v>174</v>
@@ -6113,20 +6113,20 @@
       <c r="G48" s="46"/>
       <c r="H48" s="46"/>
       <c r="I48" s="14" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="J48" s="16"/>
       <c r="K48" s="16"/>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="42" t="s">
+        <v>279</v>
+      </c>
+      <c r="B49" s="43" t="s">
+        <v>280</v>
+      </c>
+      <c r="C49" s="46" t="s">
         <v>281</v>
-      </c>
-      <c r="B49" s="43" t="s">
-        <v>282</v>
-      </c>
-      <c r="C49" s="46" t="s">
-        <v>283</v>
       </c>
       <c r="D49" s="26" t="s">
         <v>174</v>
@@ -6140,16 +6140,16 @@
       <c r="G49" s="45"/>
       <c r="H49" s="45"/>
       <c r="I49" s="26" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="J49" s="16" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="K49" s="16"/>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="42" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="B50" s="46"/>
       <c r="C50" s="46"/>
@@ -6166,7 +6166,7 @@
       <c r="A51" s="40"/>
       <c r="B51" s="40"/>
       <c r="C51" s="40" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="D51" s="40"/>
       <c r="E51" s="40"/>
@@ -6179,13 +6179,13 @@
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" s="42" t="s">
+        <v>284</v>
+      </c>
+      <c r="B52" s="43" t="s">
+        <v>285</v>
+      </c>
+      <c r="C52" s="48" t="s">
         <v>286</v>
-      </c>
-      <c r="B52" s="43" t="s">
-        <v>287</v>
-      </c>
-      <c r="C52" s="48" t="s">
-        <v>288</v>
       </c>
       <c r="D52" s="26" t="s">
         <v>174</v>
@@ -6199,17 +6199,17 @@
       <c r="G52" s="45"/>
       <c r="H52" s="45"/>
       <c r="I52" s="26" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" s="42" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" s="42" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
     </row>
   </sheetData>

</xml_diff>